<commit_message>
Project Plan - gantt chart with timelines
</commit_message>
<xml_diff>
--- a/docs/ProjectPlan-FamilyHealthTracker.xlsx
+++ b/docs/ProjectPlan-FamilyHealthTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75D19854-4789-4A81-864E-C7CA28880C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770E30CF-31D4-4352-B6BF-5CD0436346D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
     <t>Legend:</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Sprint 2</t>
   </si>
   <si>
-    <t>Family Health Track Interface</t>
-  </si>
-  <si>
     <t>Learning - React framework</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Final Documentation</t>
+  </si>
+  <si>
+    <t>Family Health Tracker Interface</t>
   </si>
 </sst>
 </file>
@@ -2058,7 +2058,7 @@
   <dimension ref="A1:BD44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2089,7 @@
   <sheetData>
     <row r="1" spans="1:56" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="1"/>
@@ -3063,13 +3063,13 @@
     </row>
     <row r="10" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="22"/>
       <c r="E10" s="23">
@@ -3278,12 +3278,14 @@
     </row>
     <row r="11" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="22"/>
       <c r="E11" s="23">
         <v>44137</v>
@@ -3491,12 +3493,14 @@
     </row>
     <row r="12" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D12" s="22"/>
       <c r="E12" s="23">
         <v>44137</v>
@@ -3557,12 +3561,14 @@
     </row>
     <row r="13" spans="1:56" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D13" s="22"/>
       <c r="E13" s="23">
         <v>44137</v>
@@ -3623,12 +3629,14 @@
     </row>
     <row r="14" spans="1:56" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="25"/>
       <c r="D14" s="22"/>
       <c r="E14" s="23">
         <v>44141</v>
@@ -3959,12 +3967,14 @@
     </row>
     <row r="16" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D16" s="22"/>
       <c r="E16" s="23">
         <v>44144</v>
@@ -4025,12 +4035,14 @@
     </row>
     <row r="17" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="22"/>
       <c r="E17" s="23">
         <v>44144</v>
@@ -4238,12 +4250,14 @@
     </row>
     <row r="18" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D18" s="22"/>
       <c r="E18" s="23">
         <v>44144</v>
@@ -4451,12 +4465,14 @@
     </row>
     <row r="19" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D19" s="22"/>
       <c r="E19" s="23">
         <v>44144</v>
@@ -4517,12 +4533,14 @@
     </row>
     <row r="20" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="25"/>
+        <v>39</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D20" s="22"/>
       <c r="E20" s="23">
         <v>44149</v>
@@ -4832,12 +4850,14 @@
     </row>
     <row r="22" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="25"/>
+      <c r="C22" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D22" s="22"/>
       <c r="E22" s="23">
         <v>44151</v>
@@ -5045,12 +5065,14 @@
     </row>
     <row r="23" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="25"/>
+      <c r="C23" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D23" s="22"/>
       <c r="E23" s="23">
         <v>44151</v>
@@ -5258,12 +5280,14 @@
     </row>
     <row r="24" spans="1:56" s="2" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="25"/>
+        <v>39</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D24" s="22"/>
       <c r="E24" s="23">
         <v>44156</v>
@@ -5471,12 +5495,14 @@
     </row>
     <row r="25" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="25"/>
+      <c r="C25" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D25" s="22"/>
       <c r="E25" s="23">
         <v>44156</v>
@@ -5891,12 +5917,14 @@
     </row>
     <row r="27" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="25"/>
+      <c r="C27" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D27" s="22"/>
       <c r="E27" s="23">
         <v>44158</v>
@@ -6104,12 +6132,14 @@
     </row>
     <row r="28" spans="1:56" s="2" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="25"/>
+      <c r="C28" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D28" s="22"/>
       <c r="E28" s="23">
         <v>44158</v>
@@ -6257,12 +6287,14 @@
     </row>
     <row r="29" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="25"/>
+      <c r="C29" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D29" s="22"/>
       <c r="E29" s="23">
         <v>44160</v>
@@ -6410,12 +6442,14 @@
     </row>
     <row r="30" spans="1:56" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="25"/>
+        <v>39</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>29</v>
+      </c>
       <c r="D30" s="22"/>
       <c r="E30" s="23">
         <v>44161</v>

</xml_diff>